<commit_message>
https://github.com/kohei-okazaki/work-3g/issues/1069  - キュー情報取込バッチがDBのapi_communication_dataへ書き込み。  - api_communication_data.transaction_id型変更  - その他軽微な修正
</commit_message>
<xml_diff>
--- a/ha-asset/02_db/DB.xlsx
+++ b/ha-asset/02_db/DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\app\git\work-3g\ha-asset\02_db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E507D38-8631-49F9-9811-7FECFE1738CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305C56FF-8B96-4594-95AB-E703CE8F0FF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="165" windowWidth="21450" windowHeight="15150" tabRatio="696" xr2:uid="{683FFC2D-57D1-4D92-A2B8-4E505AD13A7A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="696" xr2:uid="{683FFC2D-57D1-4D92-A2B8-4E505AD13A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="TABLE_LIST" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="892" uniqueCount="267">
   <si>
     <t>PRIMARY_KEY</t>
     <phoneticPr fontId="1"/>
@@ -1374,6 +1374,10 @@
   </si>
   <si>
     <t>NEWS_INFO</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>36</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1482,7 +1486,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1522,9 +1526,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
@@ -1543,9 +1544,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office テーマ">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 テーマ">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1583,7 +1584,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1689,7 +1690,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1831,7 +1832,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1842,10 +1843,10 @@
   <dimension ref="A1:M152"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.4"/>
@@ -2023,7 +2024,7 @@
         <v>179</v>
       </c>
       <c r="J5" s="1"/>
-      <c r="K5" s="12" t="s">
+      <c r="K5" s="1" t="s">
         <v>241</v>
       </c>
       <c r="L5" s="1"/>
@@ -3077,10 +3078,12 @@
       <c r="H43" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="I43" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="J43" s="1"/>
+      <c r="I43" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J43" s="12" t="s">
+        <v>266</v>
+      </c>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
       <c r="M43" s="1"/>
@@ -3124,7 +3127,9 @@
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
+      <c r="F45" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G45" s="1" t="s">
         <v>181</v>
       </c>
@@ -3153,7 +3158,9 @@
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
+      <c r="F46" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G46" s="1" t="s">
         <v>174</v>
       </c>
@@ -3448,7 +3455,7 @@
         <v>179</v>
       </c>
       <c r="J56" s="1"/>
-      <c r="K56" s="12" t="s">
+      <c r="K56" s="1" t="s">
         <v>241</v>
       </c>
       <c r="L56" s="1"/>
@@ -4154,34 +4161,34 @@
       </c>
       <c r="M80" s="1"/>
     </row>
-    <row r="81" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="12" t="s">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A81" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="C81" s="12"/>
-      <c r="D81" s="12"/>
-      <c r="E81" s="12"/>
-      <c r="F81" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G81" s="12" t="s">
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G81" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H81" s="12" t="s">
+      <c r="H81" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I81" s="12" t="s">
+      <c r="I81" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="J81" s="12"/>
-      <c r="K81" s="12" t="s">
+      <c r="J81" s="1"/>
+      <c r="K81" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="L81" s="12"/>
-      <c r="M81" s="12"/>
+      <c r="L81" s="1"/>
+      <c r="M81" s="1"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A82" s="1" t="s">
@@ -4305,34 +4312,34 @@
       </c>
       <c r="M85" s="1"/>
     </row>
-    <row r="86" spans="1:13" s="13" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="12" t="s">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A86" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B86" s="12" t="s">
+      <c r="B86" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="C86" s="12"/>
-      <c r="D86" s="12"/>
-      <c r="E86" s="12"/>
-      <c r="F86" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="G86" s="12" t="s">
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G86" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="H86" s="12" t="s">
+      <c r="H86" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="I86" s="12" t="s">
+      <c r="I86" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="J86" s="12"/>
-      <c r="K86" s="12" t="s">
+      <c r="J86" s="1"/>
+      <c r="K86" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="L86" s="12"/>
-      <c r="M86" s="12"/>
+      <c r="L86" s="1"/>
+      <c r="M86" s="1"/>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.4">
       <c r="A87" s="1" t="s">
@@ -4444,7 +4451,7 @@
         <v>179</v>
       </c>
       <c r="J90" s="1"/>
-      <c r="K90" s="12" t="s">
+      <c r="K90" s="1" t="s">
         <v>241</v>
       </c>
       <c r="L90" s="1"/>
@@ -4761,7 +4768,7 @@
         <v>179</v>
       </c>
       <c r="J101" s="1"/>
-      <c r="K101" s="12" t="s">
+      <c r="K101" s="1" t="s">
         <v>241</v>
       </c>
       <c r="L101" s="1"/>

</xml_diff>